<commit_message>
Adding select2. Added another data point and hooked up some APIs so that you can actually search stuff.
</commit_message>
<xml_diff>
--- a/data/cocktails.xlsx
+++ b/data/cocktails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>The Last Word</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Shake vigorously with ice. Strain into a g{cocktail glass} and garnish with lime twist.</t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>Shake with ice for a long time. Strain into a chilled g{cocktail glass}.</t>
+  </si>
+  <si>
+    <t>dry gin, green chartreuse, dry vermouth, absinthe, orange bitters</t>
+  </si>
+  <si>
+    <t>q{1.5} u{oz} dry gin | q{1/2} u{oz} dry vermouth | q{1/2} u{oz} green Chartreuse | q{1} u{tsp} absinthe | q{1-2} u{dashes} orange bitters</t>
   </si>
 </sst>
 </file>
@@ -402,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -433,6 +445,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Adding super-basic Backbone list view.
</commit_message>
<xml_diff>
--- a/data/cocktails.xlsx
+++ b/data/cocktails.xlsx
@@ -39,10 +39,10 @@
     <t>Ivy</t>
   </si>
   <si>
+    <t>gin, green chartreuse, dry vermouth, absinthe, orange bitters</t>
+  </si>
+  <si>
     <t>Shake with ice for a long time. Strain into a chilled g{cocktail glass}.</t>
-  </si>
-  <si>
-    <t>dry gin, green chartreuse, dry vermouth, absinthe, orange bitters</t>
   </si>
   <si>
     <t>q{1.5} u{oz} dry gin | q{1/2} u{oz} dry vermouth | q{1/2} u{oz} green Chartreuse | q{1} u{tsp} absinthe | q{1-2} u{dashes} orange bitters</t>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -450,13 +450,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements to inspection view
- added gross string-parsing to the inspect view to split out quantities and units
- added Handlebars helper to render ingredients with <span>s
- added super-basic styling to differentiate
- updated xlsx to newer format
- extracted Drink class to its own file
</commit_message>
<xml_diff>
--- a/data/cocktails.xlsx
+++ b/data/cocktails.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,24 +30,12 @@
     <t>gin, green chartreuse, maraschino liqueur, lime juice</t>
   </si>
   <si>
-    <t>q{3/4} u{oz} gin | q{3/4} u{oz} green Chartreuse | q{3/4} u{oz} maraschino liqueur | q{3/4} u{oz} lime juice | twist of lime</t>
-  </si>
-  <si>
-    <t>Shake vigorously with ice. Strain into a g{cocktail glass} and garnish with lime twist.</t>
-  </si>
-  <si>
     <t>Ivy</t>
   </si>
   <si>
     <t>gin, green chartreuse, dry vermouth, absinthe, orange bitters</t>
   </si>
   <si>
-    <t>Shake with ice for a long time. Strain into a chilled g{cocktail glass}.</t>
-  </si>
-  <si>
-    <t>q{1.5} u{oz} dry gin | q{1/2} u{oz} dry vermouth | q{1/2} u{oz} green Chartreuse | q{1} u{tsp} absinthe | q{1-2} u{dashes} orange bitters</t>
-  </si>
-  <si>
     <t>Caipirinha</t>
   </si>
   <si>
@@ -58,13 +45,25 @@
     <t>What to do about foreign characters like ç? What about common ingredients like sugar?</t>
   </si>
   <si>
-    <t>q{1} u{lime}, cut into eighths | q{1} u{tsp} sugar | q{2} u{oz} cachaça</t>
-  </si>
-  <si>
     <t>Proper Brazilian Caipirinhas are unmeasured and the glass is simply filled with cachaça after the ice is added.</t>
   </si>
   <si>
-    <t>Muddle lime and sugar in a g{lowball glass} until the lims is juiced. Fill to brim with crushed ice and add cachaça. Garnish with sugar cane.</t>
+    <t>Shake vigorously with ice. Strain into a {gcocktail glass} and garnish with lime twist.</t>
+  </si>
+  <si>
+    <t>Shake with ice for a long time. Strain into a chilled {gcocktail glass}.</t>
+  </si>
+  <si>
+    <t>Muddle lime and sugar in a {glowball glass} until the lime is juiced. Fill to brim with crushed ice and add cachaça. Garnish with sugar cane.</t>
+  </si>
+  <si>
+    <t>{q3/4}{uoz} gin | {q3/4}{uoz} green Chartreuse | {q3/4}{uoz} maraschino liqueur | {q3/4}{uoz} lime juice | twist of lime</t>
+  </si>
+  <si>
+    <t>{q1} {ulime}, cut into eighths | {q1}{utsp} sugar | {q2}{uoz} cachaça</t>
+  </si>
+  <si>
+    <t>{q1.5}{uoz} dry gin | {q1/2}{uoz} dry vermouth | {q1/2}{uoz} green Chartreuse | {q1}{utsp} absinthe | {q1-2} {udashes} orange bitters</t>
   </si>
 </sst>
 </file>
@@ -436,7 +435,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -456,10 +455,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -467,36 +466,36 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing format of data to have one ingredient per cell and inline tags for that ingredient.
</commit_message>
<xml_diff>
--- a/data/cocktails.xlsx
+++ b/data/cocktails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>The Last Word</t>
   </si>
@@ -27,21 +27,12 @@
     <t>Needs tweaking.</t>
   </si>
   <si>
-    <t>gin, green chartreuse, maraschino liqueur, lime juice</t>
-  </si>
-  <si>
     <t>Ivy</t>
   </si>
   <si>
-    <t>gin, green chartreuse, dry vermouth, absinthe, orange bitters</t>
-  </si>
-  <si>
     <t>Caipirinha</t>
   </si>
   <si>
-    <t>cachaca, lime, sugar</t>
-  </si>
-  <si>
     <t>What to do about foreign characters like ç? What about common ingredients like sugar?</t>
   </si>
   <si>
@@ -57,23 +48,69 @@
     <t>Muddle lime and sugar in a {glowball glass} until the lime is juiced. Fill to brim with crushed ice and add cachaça. Garnish with sugar cane.</t>
   </si>
   <si>
-    <t>{q3/4}{uoz} gin | {q3/4}{uoz} green Chartreuse | {q3/4}{uoz} maraschino liqueur | {q3/4}{uoz} lime juice | twist of lime</t>
-  </si>
-  <si>
-    <t>{q1} {ulime}, cut into eighths | {q1}{utsp} sugar | {q2}{uoz} cachaça</t>
-  </si>
-  <si>
-    <t>{q1.5}{uoz} dry gin | {q1/2}{uoz} dry vermouth | {q1/2}{uoz} green Chartreuse | {q1}{utsp} absinthe | {q1-2} {udashes} orange bitters</t>
+    <t>twist of lime</t>
+  </si>
+  <si>
+    <t>{q1-2} {udashes} orange bitters</t>
+  </si>
+  <si>
+    <t>gin | {q3/4}{uoz} gin</t>
+  </si>
+  <si>
+    <t>dry gin | {q1.5}{uoz} dry gin</t>
+  </si>
+  <si>
+    <t>lime | {q1} {ulime}, cut into eighths</t>
+  </si>
+  <si>
+    <t>green chartreuse | {q3/4}{uoz} green Chartreuse</t>
+  </si>
+  <si>
+    <t>dry vermouth | {q1/2}{uoz} dry vermouth</t>
+  </si>
+  <si>
+    <t>sugar | {q1}{utsp} sugar</t>
+  </si>
+  <si>
+    <t>maraschino liqueur | {q3/4}{uoz} maraschino liqueur</t>
+  </si>
+  <si>
+    <t>green chartreuse | {q1/2}{uoz} green Chartreuse</t>
+  </si>
+  <si>
+    <t>cachaca | {q2}{uoz} cachaça</t>
+  </si>
+  <si>
+    <t>lime juice | {q3/4}{uoz} lime juice</t>
+  </si>
+  <si>
+    <t>absinthe | {q1}{utsp} absinthe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,13 +133,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,74 +485,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.83203125" customWidth="1"/>
-    <col min="4" max="4" width="61.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="30.5" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>